<commit_message>
data: add 2023-05-29 notices
</commit_message>
<xml_diff>
--- a/data/position_notices/2023-05-26.xlsx
+++ b/data/position_notices/2023-05-26.xlsx
@@ -464,41 +464,41 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>股票名称</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>股票代码</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>公告标题</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>公告日期</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>公告发布时间</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>公告附件</t>
         </is>
@@ -507,32 +507,32 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ST大集</t>
+          <t>ST时万</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>000564</t>
+          <t>600241</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ST大集:2022年年度股东大会决议公告</t>
+          <t>ST时万:辽宁时代万恒股份有限公司关于撤销其他风险警示暨停牌的公告</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2023-05-27 00:00:00</t>
+          <t>2023-05-30 00:00:00</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2023-05-26 18:06:00:000</t>
-        </is>
-      </c>
-      <c r="F2" s="2" t="inlineStr">
-        <is>
-          <t>https://pdf.dfcfw.com/pdf/H2_AN202305261587293532_1.pdf?1685124360000.pdf</t>
+          <t>2023-05-29 18:47:58:000</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305291587340569_1.pdf?1685386082000.pdf</t>
         </is>
       </c>
     </row>
@@ -549,7 +549,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ST大集:关于供销大集集团股份有限公司2022年年度股东大会的法律意见书</t>
+          <t>ST大集:2022年年度股东大会决议公告</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -559,29 +559,29 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2023-05-26 18:05:41:000</t>
-        </is>
-      </c>
-      <c r="F3" s="2" t="inlineStr">
-        <is>
-          <t>https://pdf.dfcfw.com/pdf/H2_AN202305261587293505_1.pdf?1685124360000.pdf</t>
+          <t>2023-05-26 18:06:00:000</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305261587293532_1.pdf?1685302108000.pdf</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>*ST莫高</t>
+          <t>ST大集</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>600543</t>
+          <t>000564</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>*ST莫高:莫高股份关于2022年度暨2023年第一季度业绩暨分红说明会召开情况的公告</t>
+          <t>ST大集:关于供销大集集团股份有限公司2022年年度股东大会的法律意见书</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -591,187 +591,433 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2023-05-26 15:33:02:000</t>
-        </is>
-      </c>
-      <c r="F4" s="2" t="inlineStr">
-        <is>
-          <t>https://pdf.dfcfw.com/pdf/H2_AN202305261587287498_1.pdf?1685124392000.pdf</t>
+          <t>2023-05-26 18:05:41:000</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305261587293505_1.pdf?1685124360000.pdf</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>佳禾智能</t>
+          <t>*ST碳元</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>300793</t>
+          <t>603133</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>佳禾智能:关于特定股东减持时间过半未减持股份的公告</t>
+          <t>*ST碳元:碳元科技股份有限公司关于终止设立控股子公司的公告</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2023-05-26 00:00:00</t>
+          <t>2023-05-30 00:00:00</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2023-05-26 17:40:04:000</t>
-        </is>
-      </c>
-      <c r="F5" s="2" t="inlineStr">
-        <is>
-          <t>https://pdf.dfcfw.com/pdf/H2_AN202305261587292362_1.pdf?1685122833000.pdf</t>
+          <t>2023-05-29 18:04:41:000</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305291587339143_1.pdf?1685383506000.pdf</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>绿动转债</t>
+          <t>*ST碳元</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>601330</t>
+          <t>603133</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>绿色动力:绿色动力环保集团股份有限公司2023年度跟踪评级报告</t>
+          <t>*ST碳元:碳元科技股份有限公司关于拟投资设立控股子公司的公告</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2023-05-27 00:00:00</t>
+          <t>2023-05-30 00:00:00</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2023-05-26 17:19:28:000</t>
-        </is>
-      </c>
-      <c r="F6" s="2" t="inlineStr">
-        <is>
-          <t>https://pdf.dfcfw.com/pdf/H2_AN202305261587291500_1.pdf?1685121792000.pdf</t>
+          <t>2023-05-29 17:24:31:000</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305291587337645_1.pdf?1685381096000.pdf</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>绿动转债</t>
+          <t>*ST碳元</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>601330</t>
+          <t>603133</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>绿色动力:关于可转换公司债券2023年度跟踪评级结果的公告</t>
+          <t>*ST碳元:碳元科技股份有限公司第四届董事会第七次会议决议公告</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2023-05-27 00:00:00</t>
+          <t>2023-05-30 00:00:00</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2023-05-26 17:17:09:000</t>
-        </is>
-      </c>
-      <c r="F7" s="2" t="inlineStr">
-        <is>
-          <t>https://pdf.dfcfw.com/pdf/H2_AN202305261587291499_1.pdf?1685122697000.pdf</t>
+          <t>2023-05-29 17:25:04:000</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305291587337644_1.pdf?1685381096000.pdf</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>伊利股份</t>
+          <t>*ST碳元</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>600887</t>
+          <t>603133</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>伊利股份:内蒙古伊利实业集团股份有限公司关于调整2022年度利润分配现金分红总额的公告</t>
+          <t>*ST碳元:碳元科技股份有限公司关于全资子公司对外投资暨签订招商引资合同书的公告</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2023-05-27 00:00:00</t>
+          <t>2023-05-30 00:00:00</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2023-05-26 18:04:49:000</t>
-        </is>
-      </c>
-      <c r="F8" s="2" t="inlineStr">
-        <is>
-          <t>https://pdf.dfcfw.com/pdf/H2_AN202305261587293447_1.pdf?1685124532000.pdf</t>
+          <t>2023-05-29 17:25:04:000</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305291587337643_1.pdf?1685381096000.pdf</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>*ST碳元</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>603133</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>*ST碳元:碳元科技股份有限公司关于召开2023年第三次临时股东大会的通知</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2023-05-30 00:00:00</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2023-05-29 17:25:04:000</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305291587337642_1.pdf?1685381096000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>*ST莫高</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>600543</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>*ST莫高:莫高股份关于2022年度暨2023年第一季度业绩暨分红说明会召开情况的公告</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2023-05-27 00:00:00</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2023-05-26 15:33:02:000</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305261587287498_1.pdf?1685124392000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>佳禾智能</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>300793</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>佳禾智能:关于特定股东减持时间过半未减持股份的公告</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2023-05-26 00:00:00</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2023-05-26 17:40:04:000</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305261587292362_1.pdf?1685122833000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>孚日转债</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>002083</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>孚日股份:关于召开2023年第一次临时股东大会的提示性公告</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2023-05-30 00:00:00</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2023-05-29 15:40:56:000</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305291587333839_1.pdf?1685394605000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>绿动转债</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>601330</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>绿色动力:绿色动力环保集团股份有限公司2023年度跟踪评级报告</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2023-05-27 00:00:00</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2023-05-26 17:19:28:000</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305261587291500_1.pdf?1685121792000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>绿动转债</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>601330</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>绿色动力:关于可转换公司债券2023年度跟踪评级结果的公告</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2023-05-27 00:00:00</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2023-05-26 17:17:09:000</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305261587291499_1.pdf?1685305345000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>ST广珠</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>600382</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>ST广珠:广东明珠集团股份有限公司关于控股股东及其一致行动人部分股份质押及部分股份解除质押的公告</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2023-05-30 00:00:00</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2023-05-29 18:49:44:000</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305291587340878_1.pdf?1685386208000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
           <t>伊利股份</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B16" t="inlineStr">
         <is>
           <t>600887</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>伊利股份:内蒙古伊利实业集团股份有限公司关于调整2022年度利润分配现金分红总额的公告</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2023-05-27 00:00:00</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2023-05-26 18:04:49:000</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305261587293447_1.pdf?1685124532000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>伊利股份</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>600887</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
         <is>
           <t>伊利股份:内蒙古伊利实业集团股份有限公司关于股份回购实施结果暨股份变动公告</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>2023-05-27 00:00:00</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>2023-05-26 18:04:49:000</t>
         </is>
       </c>
-      <c r="F9" s="2" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t>https://pdf.dfcfw.com/pdf/H2_AN202305261587293446_1.pdf?1685124301000.pdf</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F2" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F3" r:id="rId2"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F4" r:id="rId3"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F5" r:id="rId4"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F6" r:id="rId5"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F7" r:id="rId6"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F8" r:id="rId7"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F9" r:id="rId8"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -781,7 +1027,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -809,75 +1055,135 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ST大集</t>
+          <t>ST时万</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>000564</t>
+          <t>600241</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>*ST莫高</t>
+          <t>ST大集</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>600543</t>
+          <t>000564</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>佳禾智能</t>
+          <t>*ST碳元</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>300793</t>
+          <t>603133</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>绿动转债</t>
+          <t>*ST莫高</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>601330</t>
+          <t>600543</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>佳禾智能</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>300793</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>孚日转债</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>002083</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>绿动转债</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>601330</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>ST广珠</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>600382</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t>伊利股份</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>600887</t>
         </is>
       </c>
-      <c r="C6" t="n">
+      <c r="C10" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>